<commit_message>
Añadido un nuevo párrafo y el tamaño de la letra
</commit_message>
<xml_diff>
--- a/Códigos Git por videos.xlsx
+++ b/Códigos Git por videos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t xml:space="preserve">Curso Git</t>
   </si>
@@ -125,6 +125,27 @@
   </si>
   <si>
     <t xml:space="preserve">Guardar y salir de vim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git remote add origin https://github.com/Angela1094/CursoGit.git + tecla enter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subir el repositorio a Github</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$ git push origin master </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si no sale con el comando anterior el usuario y contraseña para subir el repositorio. Sirve para actualizar los repositorios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Video 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git pull</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detecta cambios que hemos hecho en GitHub</t>
   </si>
 </sst>
 </file>
@@ -200,13 +221,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -226,13 +251,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.87"/>
   </cols>
@@ -381,10 +406,37 @@
         <v>34</v>
       </c>
     </row>
+    <row r="21" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>